<commit_message>
Fix Cost Models, Incorporate Job.xlsx
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Luna Workspace\MachineSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SingleMachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Sub-Assy</t>
   </si>
@@ -170,12 +170,21 @@
   <si>
     <t>A45</t>
   </si>
+  <si>
+    <t>Fixed Cost</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +238,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -394,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -450,6 +467,45 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -468,44 +524,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,111 +834,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="25" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28" t="s">
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="27" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="31" t="s">
+    <row r="2" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="35" t="s">
+      <c r="M2" s="23"/>
+      <c r="N2" s="26" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="29"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="29"/>
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="20"/>
       <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="36"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="27"/>
       <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="29"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="30"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
@@ -928,7 +959,7 @@
       <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="30"/>
+      <c r="J4" s="21"/>
       <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
@@ -938,12 +969,18 @@
       <c r="M4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="37"/>
+      <c r="N4" s="28"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="30"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="P4" s="21"/>
+      <c r="Q4" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -991,9 +1028,15 @@
       <c r="P5" s="10">
         <v>66000</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="Q5" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R5" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
       <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
@@ -1039,9 +1082,15 @@
       <c r="P6" s="10">
         <v>14000</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="Q6" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R6" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
       <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1087,9 +1136,15 @@
       <c r="P7" s="10">
         <v>48000</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="Q7" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R7" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
       <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1135,9 +1190,15 @@
       <c r="P8" s="10">
         <v>27000</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="Q8" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R8" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1185,9 +1246,15 @@
       <c r="P9" s="10">
         <v>24000</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+      <c r="Q9" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R9" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
       <c r="B10" s="7" t="s">
         <v>31</v>
       </c>
@@ -1233,9 +1300,15 @@
       <c r="P10" s="10">
         <v>36000</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
+      <c r="Q10" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R10" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
       <c r="B11" s="7" t="s">
         <v>32</v>
       </c>
@@ -1281,9 +1354,15 @@
       <c r="P11" s="10">
         <v>24000</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="Q11" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R11" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1331,9 +1410,15 @@
       <c r="P12" s="10">
         <v>54000</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="Q12" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R12" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
       <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
@@ -1379,9 +1464,15 @@
       <c r="P13" s="10">
         <v>24000</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="Q13" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R13" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -1429,9 +1520,15 @@
       <c r="P14" s="14">
         <v>36000</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="Q14" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R14" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36"/>
       <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
@@ -1477,9 +1574,15 @@
       <c r="P15" s="10">
         <v>48000</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="Q15" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R15" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36"/>
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1525,9 +1628,15 @@
       <c r="P16" s="10">
         <v>30000</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="Q16" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R16" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36"/>
       <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
@@ -1573,9 +1682,15 @@
       <c r="P17" s="10">
         <v>36000</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
+      <c r="Q17" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R17" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="37"/>
       <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
@@ -1621,8 +1736,14 @@
       <c r="P18" s="10">
         <v>30000</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q18" s="38">
+        <v>10000</v>
+      </c>
+      <c r="R18" s="38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
         <v>24</v>
@@ -1652,7 +1773,7 @@
       <c r="O19" s="8"/>
       <c r="P19" s="18"/>
     </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
         <v>25</v>
@@ -1684,13 +1805,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="L2:M3"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="F1:K1"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A13"/>
@@ -1701,6 +1815,13 @@
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:E4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="F1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>